<commit_message>
modified:   config/prompts.py 	modified:   config/settings.py 	modified:   "libs/\344\270\200\344\275\223\345\214\226\346\270\251\345\272\246\345\217\230\351\200\201\345\231\250\350\257\255\344\271\211\345\272\223.xlsx" 	modified:   main.py 	modified:   src/code_assembler/assembler.py 	modified:   src/code_assembler/assembly_prompt.txt 	modified:   src/parameter_standardizer/standardized_prompt.txt
</commit_message>
<xml_diff>
--- a/libs/一体化温度变送器语义库.xlsx
+++ b/libs/一体化温度变送器语义库.xlsx
@@ -542,7 +542,7 @@
     <t>304 SST或ASTM304L 2B 水平管道安装用</t>
   </si>
   <si>
-    <t>支架安装,2"管装,2“钢管,2''管安装,有,304水平安装支架, 2"横管安装 不锈钢材质, 2"横管安装,支架材质304SS,2″管装平板支架,带2"管支架及U型栓,带，304SS,YES</t>
+    <t>支架安装,2"管装支架,2“钢管,2''管安装,有,304水平安装支架, 2"横管安装 不锈钢材质, 2"横管安装,支架材质304SS,2″管装平板支架,带2"管支架及U型栓,带，304SS,YES</t>
   </si>
   <si>
     <t>304 SST或ASTM304L 2B 垂直管道安装用</t>
@@ -1146,7 +1146,7 @@
     <t>/N1</t>
   </si>
   <si>
-    <t>需一体化温度变送器与变送器NEPSI选项为NF2同时生效，且实际参数名称可能为英语</t>
+    <t>**注意：需一体化温度变送器与变送器NEPSI选项为NF2同时生效，且实际参数名称可能为英语</t>
   </si>
   <si>
     <t>一体化温度变送器本安证书</t>
@@ -1155,7 +1155,7 @@
     <t>/N2</t>
   </si>
   <si>
-    <t>需一体化温度变送器与变送器NEPSI选项为NS2或NS25同时生效，且实际参数名称可能为英语</t>
+    <t>**注意：需一体化温度变送器与变送器NEPSI选项为NS2或NS25同时生效，且实际参数名称可能为英语</t>
   </si>
   <si>
     <t>接线盒</t>
@@ -2597,7 +2597,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2687,15 +2687,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3055,10 +3046,10 @@
   <sheetPr/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E34"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3200,7 +3191,7 @@
       <c r="G6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="36" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3220,7 +3211,7 @@
       <c r="G7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="40"/>
+      <c r="I7" s="37"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="13"/>
@@ -3230,10 +3221,10 @@
       <c r="C8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="32" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="18" t="s">
@@ -3250,7 +3241,7 @@
       <c r="D9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="32" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="18" t="s">
@@ -3309,7 +3300,7 @@
       <c r="C12" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="35" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -3493,7 +3484,7 @@
       <c r="C22" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="32" t="s">
         <v>83</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -3511,7 +3502,7 @@
       <c r="C23" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="32" t="s">
         <v>88</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -3525,7 +3516,7 @@
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="32" t="s">
         <v>91</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -3539,7 +3530,7 @@
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="32" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -3553,7 +3544,7 @@
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="32" t="s">
         <v>97</v>
       </c>
       <c r="E26" s="11" t="s">
@@ -3567,7 +3558,7 @@
       <c r="A27" s="13"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="32" t="s">
         <v>100</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -3585,7 +3576,7 @@
       <c r="C28" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="32" t="s">
         <v>105</v>
       </c>
       <c r="E28" s="21"/>
@@ -3599,7 +3590,7 @@
       <c r="C29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="32" t="s">
         <v>108</v>
       </c>
       <c r="E29" s="21"/>
@@ -3611,7 +3602,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="32" t="s">
         <v>110</v>
       </c>
       <c r="E30" s="22"/>
@@ -3645,7 +3636,7 @@
       <c r="C32" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="32" t="s">
         <v>117</v>
       </c>
       <c r="E32" s="11" t="s">
@@ -3659,7 +3650,7 @@
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="32" t="s">
         <v>120</v>
       </c>
       <c r="E33" s="20" t="s">
@@ -3733,8 +3724,8 @@
   <sheetPr/>
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -4038,7 +4029,7 @@
       <c r="C13" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="30" t="s">
         <v>170</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -4242,7 +4233,7 @@
       <c r="D22" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="30" t="s">
         <v>198</v>
       </c>
       <c r="F22" s="6" t="s">
@@ -4458,7 +4449,7 @@
       <c r="F32" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G32" s="34" t="s">
+      <c r="G32" s="31" t="s">
         <v>166</v>
       </c>
       <c r="H32" s="3"/>
@@ -4476,10 +4467,10 @@
       <c r="C33" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="33" t="s">
         <v>217</v>
       </c>
       <c r="F33" s="5">
@@ -4805,7 +4796,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" customFormat="1" ht="43.2" spans="1:9">
+    <row r="48" customFormat="1" ht="115.2" spans="1:9">
       <c r="A48" s="3" t="s">
         <v>127</v>
       </c>
@@ -4978,7 +4969,7 @@
       <c r="D55" s="17"/>
     </row>
     <row r="72" spans="3:3">
-      <c r="C72" s="37"/>
+      <c r="C72" s="34"/>
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I54" etc:filterBottomFollowUsedRange="0">
@@ -5016,7 +5007,7 @@
   <sheetPr/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="C21" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -5313,7 +5304,7 @@
       <c r="E13" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G13" s="18" t="s">
@@ -5334,7 +5325,7 @@
       <c r="E14" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G14" s="18" t="s">
@@ -5355,7 +5346,7 @@
       <c r="E15" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G15" s="18" t="s">
@@ -5376,7 +5367,7 @@
       <c r="E16" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G16" s="18" t="s">
@@ -5397,7 +5388,7 @@
       <c r="E17" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G17" s="18" t="s">
@@ -5418,7 +5409,7 @@
       <c r="E18" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="F18" s="41" t="s">
+      <c r="F18" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G18" s="18" t="s">
@@ -5439,7 +5430,7 @@
       <c r="E19" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G19" s="18" t="s">
@@ -5460,10 +5451,10 @@
       <c r="E20" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="39" t="s">
         <v>328</v>
       </c>
       <c r="H20" s="3"/>
@@ -5481,10 +5472,10 @@
       <c r="E21" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="39" t="s">
         <v>331</v>
       </c>
       <c r="H21" s="3"/>
@@ -5500,7 +5491,7 @@
       <c r="E22" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="38" t="s">
         <v>308</v>
       </c>
       <c r="G22" s="18" t="s">
@@ -5586,7 +5577,7 @@
       <c r="E26" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="39" t="s">
         <v>262</v>
       </c>
     </row>
@@ -5630,7 +5621,7 @@
       <c r="G28" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="I28" s="30" t="s">
+      <c r="I28" s="12" t="s">
         <v>354</v>
       </c>
     </row>
@@ -5647,7 +5638,7 @@
       <c r="G29" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="I29" s="31"/>
+      <c r="I29" s="13"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="13"/>
@@ -5662,7 +5653,7 @@
       <c r="G30" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="I30" s="31"/>
+      <c r="I30" s="13"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="13"/>
@@ -5677,7 +5668,7 @@
       <c r="G31" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="I31" s="31"/>
+      <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="13"/>
@@ -5692,7 +5683,7 @@
       <c r="G32" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="I32" s="31"/>
+      <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="13"/>
@@ -5707,7 +5698,7 @@
       <c r="G33" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="I33" s="31"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="17"/>
@@ -5722,7 +5713,7 @@
       <c r="G34" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="I34" s="32"/>
+      <c r="I34" s="17"/>
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I34" etc:filterBottomFollowUsedRange="0">
@@ -5757,7 +5748,7 @@
   <sheetPr/>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="B35" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="E40" sqref="E40:E46"/>
     </sheetView>
   </sheetViews>
@@ -6033,7 +6024,7 @@
         <v>382</v>
       </c>
       <c r="F13" s="25"/>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="39" t="s">
         <v>383</v>
       </c>
       <c r="H13" s="3"/>
@@ -6050,7 +6041,7 @@
         <v>385</v>
       </c>
       <c r="F14" s="25"/>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="39" t="s">
         <v>386</v>
       </c>
       <c r="H14" s="3"/>
@@ -6067,7 +6058,7 @@
         <v>388</v>
       </c>
       <c r="F15" s="25"/>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="39" t="s">
         <v>389</v>
       </c>
       <c r="H15" s="3"/>
@@ -6084,7 +6075,7 @@
         <v>391</v>
       </c>
       <c r="F16" s="25"/>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="39" t="s">
         <v>392</v>
       </c>
       <c r="H16" s="3"/>
@@ -6101,7 +6092,7 @@
         <v>393</v>
       </c>
       <c r="F17" s="25"/>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="39" t="s">
         <v>332</v>
       </c>
       <c r="H17" s="3"/>
@@ -6468,7 +6459,7 @@
         <v>348</v>
       </c>
       <c r="F36" s="28"/>
-      <c r="G36" s="42" t="s">
+      <c r="G36" s="39" t="s">
         <v>262</v>
       </c>
       <c r="H36" s="3"/>
@@ -6510,7 +6501,7 @@
         <v>340</v>
       </c>
       <c r="F38" s="29"/>
-      <c r="G38" s="42" t="s">
+      <c r="G38" s="39" t="s">
         <v>439</v>
       </c>
       <c r="H38" s="11" t="s">
@@ -6529,7 +6520,7 @@
       <c r="D39" s="16"/>
       <c r="E39" s="17"/>
       <c r="F39" s="29"/>
-      <c r="G39" s="42" t="s">
+      <c r="G39" s="39" t="s">
         <v>439</v>
       </c>
       <c r="H39" s="11" t="s">
@@ -7061,7 +7052,7 @@
         <v>446</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="39" t="s">
         <v>262</v>
       </c>
       <c r="H17" s="3"/>
@@ -7320,7 +7311,7 @@
         <v>454</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="39" t="s">
         <v>262</v>
       </c>
       <c r="H4" s="3"/>
@@ -7568,7 +7559,7 @@
         <v>446</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="39" t="s">
         <v>262</v>
       </c>
       <c r="H4" s="3"/>
@@ -7725,7 +7716,7 @@
         <v>327</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="39" t="s">
         <v>328</v>
       </c>
       <c r="H13" s="3"/>
@@ -7742,7 +7733,7 @@
         <v>330</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="39" t="s">
         <v>331</v>
       </c>
       <c r="H14" s="3"/>
@@ -8019,7 +8010,7 @@
         <v>446</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="39" t="s">
         <v>262</v>
       </c>
       <c r="H4" s="3"/>
@@ -8101,7 +8092,7 @@
         <v>382</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="39" t="s">
         <v>383</v>
       </c>
       <c r="H8" s="3"/>
@@ -8118,7 +8109,7 @@
         <v>385</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="39" t="s">
         <v>386</v>
       </c>
       <c r="H9" s="3"/>
@@ -8135,7 +8126,7 @@
         <v>388</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="39" t="s">
         <v>389</v>
       </c>
       <c r="H10" s="3"/>
@@ -8152,7 +8143,7 @@
         <v>391</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="39" t="s">
         <v>392</v>
       </c>
       <c r="H11" s="3"/>
@@ -8169,7 +8160,7 @@
         <v>393</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="39" t="s">
         <v>332</v>
       </c>
       <c r="H12" s="3"/>

</xml_diff>

<commit_message>
modified:   config/settings.py 	modified:   "libs/\344\270\200\344\275\223\345\214\226\346\270\251\345\272\246\345\217\230\351\200\201\345\231\250\350\257\255\344\271\211\345\272\223.xlsx"     deleted:    scripts/__init__.py 	modified:   src/code_assembler/assembler.py 	modified:   src/code_assembler/assembly_prompt.txt 	modified:   src/parameter_standardizer/standardized_prompt.txt
</commit_message>
<xml_diff>
--- a/libs/一体化温度变送器语义库.xlsx
+++ b/libs/一体化温度变送器语义库.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10500" tabRatio="511"/>
+    <workbookView windowWidth="23040" windowHeight="10500" tabRatio="511" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="变送器部分" sheetId="2" r:id="rId1"/>
@@ -329,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="502">
   <si>
     <t>元器件部位</t>
   </si>
@@ -635,7 +635,7 @@
     <t>高防腐涂层</t>
   </si>
   <si>
-    <t>环氧漆；防腐涂层</t>
+    <t>环氧漆；防腐涂层；满足海边盐雾腐蚀涂层C5防腐</t>
   </si>
   <si>
     <t>/X2</t>
@@ -1063,7 +1063,7 @@
     <t>连接螺纹</t>
   </si>
   <si>
-    <t>传感器螺纹;连接规格；Connection Specification；螺纹规格；过程连接尺寸；连接方式；Connection Type；安装形式； MOUNTING STYLE；测温元件与保护套管连接方式；过程连接； Process Connection；过程连接形式；Process Conn；螺纹接口尺寸；Thread Size；安装固定方式；MOUNTING STYLE；连接尺寸；Connection Size；连接规格 Conn. Size &amp; Rating；与温度计套管连接；Conn. With TW；固定装置；过程连接螺纹；与温度计套管连接形式；Connection with TW；Stem Connection with Thermowell；插杆与外保护套管连接；过程连接形式；Process Connection Type；过程连接规格；PROCESS CONN. SIZE；过程接口；Conn. w/TW 与温度计套管连接；过程连接形式及等级；Process Conn. Style &amp;Rating；元件连接尺寸；Internal Conn. Size；Temp.Element Conn. Size；温度元件接头尺寸；接类型及尺寸；Connection Type and Size；保护管连接形式 STEM CONN. TYPE；与外套管连接；CONNECTED WITH THERMOWELL；元件与套管螺纹连接规格；Thread Size；温度元件接头尺寸；Temperature Element Connection Size；元件与保护管连接；测温元件连接尺寸；</t>
+    <t>传感器螺纹;过程连接形式 Process Conn.；连接规格；Connection Specification；螺纹规格；过程连接尺寸；连接方式；Connection Type；安装形式； MOUNTING STYLE；测温元件与保护套管连接方式；过程连接； Process Connection；过程连接形式；Process Conn；螺纹接口尺寸；Thread Size；安装固定方式；MOUNTING STYLE；连接尺寸；Connection Size；连接规格 Conn. Size &amp; Rating；与温度计套管连接；Conn. With TW；固定装置；过程连接螺纹；与温度计套管连接形式；Connection with TW；Stem Connection with Thermowell；插杆与外保护套管连接；过程连接形式；Process Connection Type；过程连接规格；PROCESS CONN. SIZE；过程接口；Conn. w/TW 与温度计套管连接；过程连接形式及等级；Process Conn. Style &amp;Rating；元件连接尺寸；Internal Conn. Size；Temp.Element Conn. Size；温度元件接头尺寸；接类型及尺寸；Connection Type and Size；保护管连接形式 STEM CONN. TYPE；与外套管连接；CONNECTED WITH THERMOWELL；元件与套管螺纹连接规格；Thread Size；温度元件接头尺寸；Temperature Element Connection Size；元件与保护管连接；测温元件连接尺寸；</t>
   </si>
   <si>
     <t>无；NA.</t>
@@ -1507,6 +1507,9 @@
     <t>TG-L</t>
   </si>
   <si>
+    <t>Tapered Type；Solid hole, tapered；Tapered from drilled barstock；整体钻孔锥型；Tapered；单端钻孔锥型套管；法兰连接整体锥型钻孔；法兰式锥形整体钻孔外套管；钢棒整体钻孔锥形套管；固定法兰式整体钻孔锥形保护套管；固定法兰锥形整体钻孔式；加强型锥型整体钻孔；锥形；一体化整体钻孔锥形法兰套管；整体锥形套管；整体锥形钻孔；整体钻孔式的锥形套管；整体钻孔锥形；整体钻孔锥形保护管；整体钻孔锥形管；整体钻孔锥形套管；整钻锥形；锥形整体钻孔；锥形整体钻孔式套管；整体钻孔保护管；全透焊整体钻孔锥形法兰套管</t>
+  </si>
+  <si>
     <t>TG-K</t>
   </si>
   <si>
@@ -1694,6 +1697,9 @@
   </si>
   <si>
     <t>-□□</t>
+  </si>
+  <si>
+    <t>直接使用用户提供的数值</t>
   </si>
   <si>
     <t>焊接安装保护管</t>
@@ -3046,10 +3052,10 @@
   <sheetPr/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3682,7 +3688,7 @@
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I34" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
-  <mergeCells count="28">
+  <mergeCells count="27">
     <mergeCell ref="A4:A21"/>
     <mergeCell ref="A22:A34"/>
     <mergeCell ref="B2:B3"/>
@@ -3708,7 +3714,6 @@
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E27:E30"/>
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="I6:I7"/>
   </mergeCells>
@@ -3724,8 +3729,8 @@
   <sheetPr/>
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5007,8 +5012,8 @@
   <sheetPr/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5719,7 +5724,7 @@
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I34" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="A27:A34"/>
     <mergeCell ref="B3:B5"/>
@@ -5728,7 +5733,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="C6:C12"/>
     <mergeCell ref="C13:C22"/>
-    <mergeCell ref="D22:D23"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D28:D34"/>
     <mergeCell ref="E22:E23"/>
@@ -5748,8 +5752,8 @@
   <sheetPr/>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:E46"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5844,11 +5848,11 @@
         <v>296</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>297</v>
+        <v>378</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="5" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -5865,7 +5869,7 @@
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -6012,20 +6016,20 @@
     <row r="13" customFormat="1" spans="1:9">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>374</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="39" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -6035,14 +6039,14 @@
       <c r="B14" s="13"/>
       <c r="C14" s="21"/>
       <c r="D14" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="39" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -6052,14 +6056,14 @@
       <c r="B15" s="13"/>
       <c r="C15" s="21"/>
       <c r="D15" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="39" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -6069,14 +6073,14 @@
       <c r="B16" s="13"/>
       <c r="C16" s="21"/>
       <c r="D16" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="39" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -6089,7 +6093,7 @@
         <v>164</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="39" t="s">
@@ -6103,14 +6107,14 @@
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" s="13"/>
       <c r="B18" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="5">
@@ -6124,10 +6128,10 @@
       <c r="B19" s="13"/>
       <c r="C19" s="21"/>
       <c r="D19" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="5">
@@ -6141,10 +6145,10 @@
       <c r="B20" s="13"/>
       <c r="C20" s="21"/>
       <c r="D20" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="5">
@@ -6175,23 +6179,23 @@
     <row r="22" customFormat="1" ht="28.8" spans="1:9">
       <c r="A22" s="13"/>
       <c r="B22" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="5">
         <v>1</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -6200,17 +6204,17 @@
       <c r="B23" s="13"/>
       <c r="C23" s="21"/>
       <c r="D23" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="5">
         <v>2</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -6219,17 +6223,17 @@
       <c r="B24" s="13"/>
       <c r="C24" s="21"/>
       <c r="D24" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="5">
         <v>3</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -6238,17 +6242,17 @@
       <c r="B25" s="13"/>
       <c r="C25" s="21"/>
       <c r="D25" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="5">
         <v>4</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -6257,17 +6261,17 @@
       <c r="B26" s="13"/>
       <c r="C26" s="21"/>
       <c r="D26" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="5">
         <v>5</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -6276,17 +6280,17 @@
       <c r="B27" s="13"/>
       <c r="C27" s="21"/>
       <c r="D27" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F27" s="25"/>
       <c r="G27" s="5">
         <v>6</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -6295,17 +6299,17 @@
       <c r="B28" s="13"/>
       <c r="C28" s="21"/>
       <c r="D28" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="5">
         <v>7</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -6314,17 +6318,17 @@
       <c r="B29" s="13"/>
       <c r="C29" s="21"/>
       <c r="D29" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="5">
         <v>8</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -6333,17 +6337,17 @@
       <c r="B30" s="13"/>
       <c r="C30" s="21"/>
       <c r="D30" s="4" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="5">
         <v>9</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -6352,17 +6356,17 @@
       <c r="B31" s="13"/>
       <c r="C31" s="21"/>
       <c r="D31" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F31" s="25"/>
       <c r="G31" s="5">
         <v>10</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -6371,17 +6375,17 @@
       <c r="B32" s="13"/>
       <c r="C32" s="21"/>
       <c r="D32" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="5">
         <v>11</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -6398,7 +6402,7 @@
         <v>166</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>257</v>
@@ -6407,16 +6411,16 @@
     <row r="34" customFormat="1" spans="1:9">
       <c r="A34" s="13"/>
       <c r="B34" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="5"/>
@@ -6426,15 +6430,15 @@
     <row r="35" customFormat="1" ht="57.6" spans="1:9">
       <c r="A35" s="13"/>
       <c r="B35" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="17"/>
       <c r="F35" s="27" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G35" s="18" t="s">
         <v>336</v>
@@ -6450,7 +6454,7 @@
         <v>346</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>165</v>
@@ -6468,7 +6472,7 @@
     <row r="37" customFormat="1" ht="43.2" spans="1:9">
       <c r="A37" s="13"/>
       <c r="B37" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>335</v>
@@ -6476,7 +6480,7 @@
       <c r="D37" s="16"/>
       <c r="E37" s="17"/>
       <c r="F37" s="27" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="G37" s="18" t="s">
         <v>336</v>
@@ -6502,12 +6506,14 @@
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="39" t="s">
-        <v>439</v>
-      </c>
-      <c r="H38" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="H38" t="s">
+        <v>441</v>
+      </c>
+      <c r="I38" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="I38" s="3"/>
     </row>
     <row r="39" customFormat="1" ht="100.8" spans="1:9">
       <c r="A39" s="17"/>
@@ -6521,12 +6527,11 @@
       <c r="E39" s="17"/>
       <c r="F39" s="29"/>
       <c r="G39" s="39" t="s">
-        <v>439</v>
-      </c>
-      <c r="H39" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="I39" s="3"/>
     </row>
     <row r="40" customFormat="1" ht="28.8" spans="1:9">
       <c r="A40" s="12" t="s">
@@ -6657,7 +6662,7 @@
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I46" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
-  <mergeCells count="23">
+  <mergeCells count="15">
     <mergeCell ref="A2:A39"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="B3:B5"/>
@@ -6669,18 +6674,10 @@
     <mergeCell ref="C6:C12"/>
     <mergeCell ref="C13:C21"/>
     <mergeCell ref="C22:C33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
     <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D46"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="E40:E46"/>
-    <mergeCell ref="F2:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F37:F46"/>
+    <mergeCell ref="H38:H39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -6742,19 +6739,19 @@
     </row>
     <row r="2" customFormat="1" ht="216" spans="1:9">
       <c r="A2" s="12" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>287</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -6952,14 +6949,14 @@
     <row r="13" customFormat="1" ht="54" customHeight="1" spans="1:9">
       <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="12" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F13" s="6">
         <v>50</v>
@@ -6968,7 +6965,7 @@
         <v>262</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -7043,13 +7040,13 @@
         <v>346</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>165</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="39" t="s">
@@ -7104,7 +7101,7 @@
         <v>358</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="13"/>
@@ -7210,7 +7207,7 @@
   <sheetPr/>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7:E10"/>
     </sheetView>
   </sheetViews>
@@ -7258,7 +7255,7 @@
     </row>
     <row r="2" customFormat="1" ht="216" spans="1:9">
       <c r="A2" s="12" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>287</v>
@@ -7284,14 +7281,14 @@
         <v>292</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -7302,13 +7299,13 @@
         <v>346</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>165</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="39" t="s">
@@ -7339,20 +7336,20 @@
     <row r="6" customFormat="1" ht="100.8" spans="1:9">
       <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>336</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>345</v>
@@ -7504,7 +7501,7 @@
     </row>
     <row r="2" customFormat="1" ht="158.4" spans="1:9">
       <c r="A2" s="12" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>291</v>
@@ -7513,10 +7510,10 @@
         <v>292</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -7539,7 +7536,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -7550,13 +7547,13 @@
         <v>346</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>165</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="39" t="s">
@@ -7568,16 +7565,16 @@
     <row r="5" customFormat="1" ht="28.8" spans="1:9">
       <c r="A5" s="13"/>
       <c r="B5" s="3" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="17"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -7585,7 +7582,7 @@
     <row r="6" customFormat="1" ht="43.2" spans="1:9">
       <c r="A6" s="13"/>
       <c r="B6" s="12" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>288</v>
@@ -7780,20 +7777,20 @@
     <row r="17" customFormat="1" ht="100.8" spans="1:9">
       <c r="A17" s="17"/>
       <c r="B17" s="3" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>336</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>345</v>
@@ -7839,7 +7836,7 @@
         <v>352</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5" t="s">
@@ -7955,7 +7952,7 @@
     </row>
     <row r="2" customFormat="1" ht="158.4" spans="1:9">
       <c r="A2" s="12" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>291</v>
@@ -7964,10 +7961,10 @@
         <v>292</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -7990,7 +7987,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -8001,13 +7998,13 @@
         <v>346</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>165</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="39" t="s">
@@ -8019,16 +8016,16 @@
     <row r="5" customFormat="1" ht="28.8" spans="1:9">
       <c r="A5" s="13"/>
       <c r="B5" s="3" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="13"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -8055,20 +8052,20 @@
     <row r="7" customFormat="1" ht="100.8" spans="1:9">
       <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>336</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>345</v>
@@ -8080,20 +8077,20 @@
     <row r="8" customFormat="1" spans="1:9">
       <c r="A8" s="13"/>
       <c r="B8" s="12" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>374</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="39" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -8103,14 +8100,14 @@
       <c r="B9" s="13"/>
       <c r="C9" s="21"/>
       <c r="D9" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="39" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -8120,14 +8117,14 @@
       <c r="B10" s="13"/>
       <c r="C10" s="21"/>
       <c r="D10" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="39" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -8137,14 +8134,14 @@
       <c r="B11" s="13"/>
       <c r="C11" s="21"/>
       <c r="D11" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="39" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -8157,7 +8154,7 @@
         <v>164</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="39" t="s">
@@ -8171,14 +8168,14 @@
     <row r="13" customFormat="1" spans="1:9">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5">
@@ -8192,10 +8189,10 @@
       <c r="B14" s="13"/>
       <c r="C14" s="21"/>
       <c r="D14" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5">
@@ -8209,10 +8206,10 @@
       <c r="B15" s="13"/>
       <c r="C15" s="21"/>
       <c r="D15" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5">
@@ -8243,23 +8240,23 @@
     <row r="17" customFormat="1" ht="28.8" spans="1:9">
       <c r="A17" s="13"/>
       <c r="B17" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5">
         <v>1</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -8268,17 +8265,17 @@
       <c r="B18" s="13"/>
       <c r="C18" s="21"/>
       <c r="D18" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5">
         <v>2</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -8287,17 +8284,17 @@
       <c r="B19" s="13"/>
       <c r="C19" s="21"/>
       <c r="D19" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5">
         <v>3</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -8306,17 +8303,17 @@
       <c r="B20" s="13"/>
       <c r="C20" s="21"/>
       <c r="D20" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5">
         <v>4</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I20" s="3"/>
     </row>
@@ -8325,17 +8322,17 @@
       <c r="B21" s="13"/>
       <c r="C21" s="21"/>
       <c r="D21" s="4" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5">
         <v>5</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -8344,17 +8341,17 @@
       <c r="B22" s="13"/>
       <c r="C22" s="21"/>
       <c r="D22" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5">
         <v>6</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -8363,17 +8360,17 @@
       <c r="B23" s="13"/>
       <c r="C23" s="21"/>
       <c r="D23" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5">
         <v>7</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -8390,7 +8387,7 @@
         <v>166</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>257</v>
@@ -8399,16 +8396,16 @@
     <row r="25" customFormat="1" spans="1:9">
       <c r="A25" s="13"/>
       <c r="B25" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -8431,7 +8428,7 @@
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>345</v>
@@ -8562,10 +8559,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -8592,46 +8589,46 @@
     </row>
     <row r="5" ht="13.5" customHeight="1" spans="2:4">
       <c r="B5" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" ht="24" spans="2:4">
       <c r="B7" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" ht="24" spans="2:4">
       <c r="B8" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" ht="24" spans="2:4">
@@ -8639,10 +8636,10 @@
         <v>172</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -8650,7 +8647,7 @@
         <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>183</v>
@@ -8661,21 +8658,21 @@
         <v>178</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" ht="24" spans="2:4">
@@ -8683,10 +8680,10 @@
         <v>181</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="14" ht="24" spans="2:4">
@@ -8694,32 +8691,32 @@
         <v>175</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="16" ht="24" spans="2:4">
       <c r="B16" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="17" spans="2:4">

</xml_diff>